<commit_message>
rice trait dictionary version 5
all the columns are displayed
</commit_message>
<xml_diff>
--- a/TD_CO_320_Rice_EN_v5.xlsx
+++ b/TD_CO_320_Rice_EN_v5.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26207"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marie-angeliquelaporte/Documents/ibp-rice-traits/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="38190" windowHeight="7500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="3" r:id="rId1"/>
@@ -13,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Template for submission'!$A$1:$AZ$286</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -11969,7 +11974,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -12047,11 +12052,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="14">
@@ -12347,125 +12347,11 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Insatisfaisant" xfId="1" builtinId="27"/>
+    <cellStyle name="Monétaire" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -12985,61 +12871,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.85546875" customWidth="1"/>
-    <col min="2" max="2" width="51.42578125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" customWidth="1"/>
+    <col min="1" max="1" width="41.83203125" customWidth="1"/>
+    <col min="2" max="2" width="51.5" style="10" customWidth="1"/>
+    <col min="3" max="3" width="9.5" customWidth="1"/>
+    <col min="4" max="4" width="37.5" customWidth="1"/>
     <col min="5" max="5" width="34" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.42578125" style="51" customWidth="1"/>
-    <col min="9" max="9" width="74.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="49.5" style="51" customWidth="1"/>
+    <col min="9" max="9" width="74.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="21"/>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>144</v>
       </c>
       <c r="H3" s="52"/>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="38" t="s">
         <v>136</v>
       </c>
       <c r="H4" s="52"/>
     </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>137</v>
       </c>
       <c r="H5" s="52"/>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>138</v>
       </c>
       <c r="H6" s="52"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>10</v>
       </c>
@@ -13047,7 +12933,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>99</v>
       </c>
@@ -13055,7 +12941,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>98</v>
       </c>
@@ -13063,7 +12949,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
@@ -13071,7 +12957,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>120</v>
       </c>
@@ -13080,7 +12966,7 @@
       </c>
       <c r="C13" s="23"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>121</v>
       </c>
@@ -13088,7 +12974,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
@@ -13096,7 +12982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>45</v>
       </c>
@@ -13104,7 +12990,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="s">
         <v>53</v>
       </c>
@@ -13112,7 +12998,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>81</v>
       </c>
@@ -13120,7 +13006,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="36" t="s">
         <v>82</v>
       </c>
@@ -13128,7 +13014,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="36" t="s">
         <v>54</v>
       </c>
@@ -13136,7 +13022,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="36" t="s">
         <v>52</v>
       </c>
@@ -13144,7 +13030,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="36" t="s">
         <v>46</v>
       </c>
@@ -13152,7 +13038,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="36" t="s">
         <v>49</v>
       </c>
@@ -13160,7 +13046,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="36" t="s">
         <v>55</v>
       </c>
@@ -13168,7 +13054,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="36" t="s">
         <v>50</v>
       </c>
@@ -13176,7 +13062,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="36" t="s">
         <v>77</v>
       </c>
@@ -13184,7 +13070,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="45" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
         <v>56</v>
       </c>
@@ -13192,7 +13078,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
         <v>57</v>
       </c>
@@ -13200,7 +13086,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>59</v>
       </c>
@@ -13208,7 +13094,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>72</v>
       </c>
@@ -13216,7 +13102,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
         <v>58</v>
       </c>
@@ -13224,7 +13110,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
         <v>63</v>
       </c>
@@ -13232,7 +13118,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="45" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>64</v>
       </c>
@@ -13240,7 +13126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>66</v>
       </c>
@@ -13248,7 +13134,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>91</v>
       </c>
@@ -13256,7 +13142,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>67</v>
       </c>
@@ -13264,7 +13150,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>69</v>
       </c>
@@ -13272,7 +13158,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>70</v>
       </c>
@@ -13280,7 +13166,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>78</v>
       </c>
@@ -13288,7 +13174,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>89</v>
       </c>
@@ -13296,13 +13182,13 @@
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="16" t="s">
         <v>3516</v>
       </c>
       <c r="B41" s="16"/>
     </row>
-    <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" s="16" t="s">
         <v>74</v>
       </c>
@@ -13310,7 +13196,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="16" t="s">
         <v>75</v>
       </c>
@@ -13318,7 +13204,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A44" s="16" t="s">
         <v>62</v>
       </c>
@@ -13326,7 +13212,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A45" s="16" t="s">
         <v>60</v>
       </c>
@@ -13334,7 +13220,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A46" s="16" t="s">
         <v>80</v>
       </c>
@@ -13342,7 +13228,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="16" t="s">
         <v>92</v>
       </c>
@@ -13350,13 +13236,13 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="16" t="s">
         <v>76</v>
       </c>
       <c r="B48" s="19"/>
     </row>
-    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
         <v>40</v>
       </c>
@@ -13364,22 +13250,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="32" t="s">
         <v>119</v>
       </c>
@@ -13387,7 +13273,7 @@
       <c r="D56" s="35"/>
       <c r="H56" s="53"/>
     </row>
-    <row r="57" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="27" t="s">
         <v>102</v>
       </c>
@@ -13409,12 +13295,12 @@
       <c r="H57" s="63"/>
       <c r="I57" s="63"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D58" s="26"/>
       <c r="H58" s="64"/>
       <c r="I58" s="55"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B59"/>
       <c r="D59" s="26" t="s">
         <v>107</v>
@@ -13428,7 +13314,7 @@
       <c r="H59" s="64"/>
       <c r="I59" s="55"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B60" s="29" t="s">
         <v>108</v>
       </c>
@@ -13450,7 +13336,7 @@
       <c r="H60" s="64"/>
       <c r="I60" s="55"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B61" s="3" t="s">
         <v>23</v>
       </c>
@@ -13473,7 +13359,7 @@
       <c r="H61" s="64"/>
       <c r="I61" s="55"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B62" s="3" t="s">
         <v>21</v>
       </c>
@@ -13497,7 +13383,7 @@
       <c r="H62" s="64"/>
       <c r="I62" s="55"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B63" s="3" t="s">
         <v>12</v>
       </c>
@@ -13521,7 +13407,7 @@
       <c r="H63" s="64"/>
       <c r="I63" s="55"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B64" s="3" t="s">
         <v>22</v>
       </c>
@@ -13545,7 +13431,7 @@
       <c r="H64" s="64"/>
       <c r="I64" s="55"/>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B65" s="4" t="s">
         <v>24</v>
       </c>
@@ -13564,7 +13450,7 @@
       <c r="H65" s="64"/>
       <c r="I65" s="55"/>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B66" s="4" t="s">
         <v>25</v>
       </c>
@@ -13584,7 +13470,7 @@
       <c r="H66" s="64"/>
       <c r="I66" s="55"/>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B67" s="4" t="s">
         <v>33</v>
       </c>
@@ -13604,7 +13490,7 @@
       <c r="H67" s="64"/>
       <c r="I67" s="64"/>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B68" s="4" t="s">
         <v>31</v>
       </c>
@@ -13624,7 +13510,7 @@
       <c r="H68" s="64"/>
       <c r="I68" s="55"/>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B69" s="4" t="s">
         <v>29</v>
       </c>
@@ -13644,7 +13530,7 @@
       <c r="H69" s="64"/>
       <c r="I69" s="55"/>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B70" s="4" t="s">
         <v>26</v>
       </c>
@@ -13664,7 +13550,7 @@
       <c r="H70" s="64"/>
       <c r="I70" s="55"/>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B71" s="4" t="s">
         <v>34</v>
       </c>
@@ -13684,7 +13570,7 @@
       <c r="H71" s="64"/>
       <c r="I71" s="55"/>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B72" s="4" t="s">
         <v>35</v>
       </c>
@@ -13702,7 +13588,7 @@
       <c r="H72" s="64"/>
       <c r="I72" s="55"/>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B73"/>
       <c r="D73" s="26" t="s">
         <v>107</v>
@@ -13716,7 +13602,7 @@
       <c r="H73" s="64"/>
       <c r="I73" s="55"/>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B74"/>
       <c r="D74" s="26" t="s">
         <v>107</v>
@@ -13730,7 +13616,7 @@
       <c r="H74" s="64"/>
       <c r="I74" s="55"/>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B75"/>
       <c r="D75" s="26" t="s">
         <v>107</v>
@@ -13744,7 +13630,7 @@
       <c r="H75" s="64"/>
       <c r="I75" s="55"/>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B76"/>
       <c r="D76" s="26" t="s">
         <v>107</v>
@@ -13758,7 +13644,7 @@
       <c r="H76" s="64"/>
       <c r="I76" s="55"/>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B77"/>
       <c r="D77" s="26" t="s">
         <v>107</v>
@@ -13772,7 +13658,7 @@
       <c r="H77" s="64"/>
       <c r="I77" s="55"/>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B78" s="17" t="s">
         <v>111</v>
       </c>
@@ -13792,7 +13678,7 @@
       <c r="H78" s="64"/>
       <c r="I78" s="55"/>
     </row>
-    <row r="79" spans="2:9" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:9" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B79" s="17" t="s">
         <v>112</v>
       </c>
@@ -13812,7 +13698,7 @@
       <c r="H79" s="64"/>
       <c r="I79" s="64"/>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B80" s="17" t="s">
         <v>32</v>
       </c>
@@ -13832,7 +13718,7 @@
       <c r="H80" s="64"/>
       <c r="I80" s="55"/>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B81"/>
       <c r="D81" s="26" t="s">
         <v>107</v>
@@ -13846,7 +13732,7 @@
       <c r="H81" s="64"/>
       <c r="I81" s="55"/>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B82"/>
       <c r="D82" s="30" t="s">
         <v>107</v>
@@ -13860,7 +13746,7 @@
       <c r="H82" s="64"/>
       <c r="I82" s="55"/>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B83" s="17" t="s">
         <v>113</v>
       </c>
@@ -13880,7 +13766,7 @@
       <c r="H83" s="64"/>
       <c r="I83" s="55"/>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B84" s="17" t="s">
         <v>27</v>
       </c>
@@ -13900,7 +13786,7 @@
       <c r="H84" s="64"/>
       <c r="I84" s="64"/>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B85" s="17" t="s">
         <v>28</v>
       </c>
@@ -13914,7 +13800,7 @@
       <c r="H85" s="64"/>
       <c r="I85" s="55"/>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B86" s="5" t="s">
         <v>114</v>
       </c>
@@ -13934,7 +13820,7 @@
       <c r="H86" s="64"/>
       <c r="I86" s="55"/>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D87" s="30" t="s">
         <v>107</v>
       </c>
@@ -13947,7 +13833,7 @@
       <c r="H87" s="64"/>
       <c r="I87" s="64"/>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B88" s="6" t="s">
         <v>36</v>
       </c>
@@ -13967,7 +13853,7 @@
       <c r="H88" s="64"/>
       <c r="I88" s="55"/>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B89" s="7" t="s">
         <v>13</v>
       </c>
@@ -13981,7 +13867,7 @@
       <c r="H89" s="64"/>
       <c r="I89" s="55"/>
     </row>
-    <row r="90" spans="2:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B90" s="6" t="s">
         <v>37</v>
       </c>
@@ -13995,7 +13881,7 @@
       <c r="H90" s="64"/>
       <c r="I90" s="55"/>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B91"/>
       <c r="D91" s="30" t="s">
         <v>107</v>
@@ -14009,7 +13895,7 @@
       <c r="H91" s="64"/>
       <c r="I91" s="55"/>
     </row>
-    <row r="92" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B92" s="5" t="s">
         <v>38</v>
       </c>
@@ -14029,7 +13915,7 @@
       <c r="H92" s="64"/>
       <c r="I92" s="55"/>
     </row>
-    <row r="93" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B93" s="5" t="s">
         <v>39</v>
       </c>
@@ -14049,7 +13935,7 @@
       <c r="H93" s="64"/>
       <c r="I93" s="55"/>
     </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B94"/>
       <c r="D94" s="30" t="s">
         <v>107</v>
@@ -14063,7 +13949,7 @@
       <c r="H94" s="64"/>
       <c r="I94" s="55"/>
     </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B95" s="6" t="s">
         <v>42</v>
       </c>
@@ -14077,7 +13963,7 @@
       <c r="H95" s="64"/>
       <c r="I95" s="55"/>
     </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B96" s="6" t="s">
         <v>14</v>
       </c>
@@ -14091,7 +13977,7 @@
       <c r="H96" s="64"/>
       <c r="I96" s="55"/>
     </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B97" s="5" t="s">
         <v>117</v>
       </c>
@@ -14110,7 +13996,7 @@
       <c r="H97" s="64"/>
       <c r="I97" s="55"/>
     </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B98"/>
       <c r="D98" s="30" t="s">
         <v>107</v>
@@ -14124,7 +14010,7 @@
       <c r="H98" s="64"/>
       <c r="I98" s="64"/>
     </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B99"/>
       <c r="D99" s="30" t="s">
         <v>107</v>
@@ -14138,7 +14024,7 @@
       <c r="H99" s="64"/>
       <c r="I99" s="64"/>
     </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B100"/>
       <c r="D100" s="30" t="s">
         <v>107</v>
@@ -14154,11 +14040,6 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -14166,60 +14047,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX284"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="AT15" sqref="AT15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" style="49" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="49" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="49" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="49" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="49" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="13" style="49" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" style="49" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.85546875" style="49" customWidth="1"/>
-    <col min="9" max="9" width="23.140625" style="49" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" style="49" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" style="49" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" style="49" customWidth="1"/>
-    <col min="13" max="13" width="50.42578125" style="49" customWidth="1"/>
-    <col min="14" max="14" width="22" style="49" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" style="49" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="46.7109375" style="49" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="24.85546875" style="49" customWidth="1"/>
+    <col min="1" max="1" width="28.5" style="49" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="49" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="49" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" style="49" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="49" customWidth="1"/>
+    <col min="6" max="6" width="13" style="49" customWidth="1"/>
+    <col min="7" max="7" width="19.83203125" style="49" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.83203125" style="49" customWidth="1"/>
+    <col min="9" max="9" width="23.1640625" style="49" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" style="49" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" style="49" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" style="49" customWidth="1"/>
+    <col min="13" max="13" width="50.5" style="49" customWidth="1"/>
+    <col min="14" max="14" width="22" style="49" customWidth="1"/>
+    <col min="15" max="15" width="13.1640625" style="49" customWidth="1"/>
+    <col min="16" max="16" width="46.6640625" style="49" customWidth="1"/>
+    <col min="17" max="17" width="24.83203125" style="49" customWidth="1"/>
     <col min="18" max="18" width="45" style="49" customWidth="1"/>
-    <col min="19" max="19" width="38.42578125" style="49" customWidth="1"/>
-    <col min="20" max="21" width="13.42578125" style="49" customWidth="1"/>
-    <col min="22" max="22" width="22.7109375" style="50" customWidth="1"/>
-    <col min="23" max="23" width="20.42578125" style="49" customWidth="1"/>
-    <col min="24" max="24" width="16.7109375" style="49" customWidth="1"/>
-    <col min="25" max="25" width="15.85546875" style="49" customWidth="1"/>
-    <col min="26" max="26" width="16.42578125" style="49" hidden="1" customWidth="1"/>
-    <col min="27" max="29" width="14" style="51" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="14" style="51" customWidth="1"/>
-    <col min="31" max="31" width="21.42578125" style="51" customWidth="1"/>
-    <col min="32" max="32" width="18.42578125" style="51" customWidth="1"/>
-    <col min="33" max="33" width="17.85546875" style="51" customWidth="1"/>
-    <col min="34" max="34" width="16.85546875" style="51" customWidth="1"/>
-    <col min="35" max="35" width="9.7109375" style="51" customWidth="1"/>
-    <col min="36" max="36" width="20.85546875" style="51" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="14" style="51" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="26.140625" style="51" hidden="1" customWidth="1"/>
-    <col min="39" max="42" width="14" style="51" hidden="1" customWidth="1"/>
-    <col min="43" max="43" width="19.85546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="32.5703125" style="49" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="15.42578125" style="49" hidden="1" customWidth="1"/>
-    <col min="46" max="46" width="18.28515625" style="49" hidden="1" customWidth="1"/>
-    <col min="47" max="47" width="17" style="49" hidden="1" customWidth="1"/>
-    <col min="48" max="48" width="15.42578125" style="49" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="38.5" style="49" customWidth="1"/>
+    <col min="20" max="21" width="13.5" style="49" customWidth="1"/>
+    <col min="22" max="22" width="22.6640625" style="50" customWidth="1"/>
+    <col min="23" max="23" width="20.5" style="49" customWidth="1"/>
+    <col min="24" max="24" width="16.6640625" style="49" customWidth="1"/>
+    <col min="25" max="25" width="15.83203125" style="49" customWidth="1"/>
+    <col min="26" max="26" width="16.5" style="49" customWidth="1"/>
+    <col min="27" max="30" width="14" style="51" customWidth="1"/>
+    <col min="31" max="31" width="21.5" style="51" customWidth="1"/>
+    <col min="32" max="32" width="18.5" style="51" customWidth="1"/>
+    <col min="33" max="33" width="17.83203125" style="51" customWidth="1"/>
+    <col min="34" max="34" width="16.83203125" style="51" customWidth="1"/>
+    <col min="35" max="35" width="9.6640625" style="51" customWidth="1"/>
+    <col min="36" max="36" width="20.83203125" style="51" customWidth="1"/>
+    <col min="37" max="37" width="14" style="51" customWidth="1"/>
+    <col min="38" max="38" width="26.1640625" style="51" customWidth="1"/>
+    <col min="39" max="42" width="14" style="51" customWidth="1"/>
+    <col min="43" max="43" width="19.83203125" style="51" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="32.5" style="49" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.5" style="49" customWidth="1"/>
+    <col min="46" max="46" width="18.33203125" style="49" customWidth="1"/>
+    <col min="47" max="47" width="17" style="49" customWidth="1"/>
+    <col min="48" max="48" width="15.5" style="49" customWidth="1"/>
     <col min="49" max="49" width="12" style="49" customWidth="1"/>
-    <col min="50" max="16384" width="11.42578125" style="49"/>
+    <col min="50" max="16384" width="11.5" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>99</v>
       </c>
@@ -14368,7 +14248,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="54"/>
       <c r="C2" s="41" t="s">
         <v>41</v>
@@ -14470,7 +14350,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="3" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="41" t="s">
         <v>41</v>
       </c>
@@ -14559,7 +14439,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="4" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="54"/>
       <c r="C4" s="41" t="s">
         <v>41</v>
@@ -14631,7 +14511,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="5" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="54"/>
       <c r="C5" s="41" t="s">
         <v>41</v>
@@ -14709,7 +14589,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="6" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="54"/>
       <c r="C6" s="41" t="s">
         <v>41</v>
@@ -14781,7 +14661,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="7" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="54"/>
       <c r="C7" s="41" t="s">
         <v>41</v>
@@ -14863,7 +14743,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="8" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="54"/>
       <c r="C8" s="41" t="s">
         <v>41</v>
@@ -14948,7 +14828,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="9" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="54"/>
       <c r="C9" s="41" t="s">
         <v>41</v>
@@ -15033,7 +14913,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="10" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="54"/>
       <c r="C10" s="41" t="s">
         <v>41</v>
@@ -15118,7 +14998,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="11" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="54"/>
       <c r="C11" s="41" t="s">
         <v>41</v>
@@ -15208,7 +15088,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="12" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="54"/>
       <c r="C12" s="41" t="s">
         <v>41</v>
@@ -15307,7 +15187,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="13" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="54"/>
       <c r="C13" s="41" t="s">
         <v>41</v>
@@ -15406,7 +15286,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="14" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="54"/>
       <c r="C14" s="41" t="s">
         <v>41</v>
@@ -15499,7 +15379,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="15" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="54"/>
       <c r="C15" s="41" t="s">
         <v>41</v>
@@ -15575,7 +15455,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="16" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="54"/>
       <c r="C16" s="41" t="s">
         <v>41</v>
@@ -15651,7 +15531,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="17" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="54"/>
       <c r="C17" s="41" t="s">
         <v>41</v>
@@ -15741,7 +15621,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="18" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="54"/>
       <c r="C18" s="41" t="s">
         <v>41</v>
@@ -15843,7 +15723,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="19" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="54"/>
       <c r="C19" s="41" t="s">
         <v>41</v>
@@ -15939,7 +15819,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="20" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="54"/>
       <c r="C20" s="41" t="s">
         <v>41</v>
@@ -16041,7 +15921,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="21" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="54"/>
       <c r="C21" s="41" t="s">
         <v>41</v>
@@ -16143,7 +16023,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="22" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="54"/>
       <c r="C22" s="41" t="s">
         <v>41</v>
@@ -16239,7 +16119,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="23" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="54"/>
       <c r="C23" s="41" t="s">
         <v>41</v>
@@ -16327,7 +16207,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="24" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="54"/>
       <c r="C24" s="41" t="s">
         <v>41</v>
@@ -16399,7 +16279,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="25" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="54"/>
       <c r="C25" s="41" t="s">
         <v>41</v>
@@ -16489,7 +16369,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="26" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="54"/>
       <c r="C26" s="41" t="s">
         <v>41</v>
@@ -16579,7 +16459,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="27" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="54"/>
       <c r="C27" s="41" t="s">
         <v>41</v>
@@ -16657,7 +16537,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="28" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="54"/>
       <c r="C28" s="41" t="s">
         <v>41</v>
@@ -16738,7 +16618,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="29" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="54"/>
       <c r="C29" s="41" t="s">
         <v>41</v>
@@ -16810,7 +16690,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="30" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="54"/>
       <c r="C30" s="41" t="s">
         <v>41</v>
@@ -16906,7 +16786,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="31" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="54"/>
       <c r="C31" s="41" t="s">
         <v>41</v>
@@ -17008,7 +16888,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="32" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="54"/>
       <c r="C32" s="41" t="s">
         <v>41</v>
@@ -17098,7 +16978,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="33" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="54"/>
       <c r="C33" s="41" t="s">
         <v>41</v>
@@ -17188,7 +17068,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="34" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="54"/>
       <c r="C34" s="41" t="s">
         <v>41</v>
@@ -17293,7 +17173,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="35" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="54"/>
       <c r="C35" s="41" t="s">
         <v>41</v>
@@ -17386,7 +17266,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="36" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="54"/>
       <c r="C36" s="41" t="s">
         <v>41</v>
@@ -17491,7 +17371,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="37" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="54"/>
       <c r="B37" s="41" t="s">
         <v>145</v>
@@ -17570,7 +17450,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="38" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="54"/>
       <c r="C38" s="41" t="s">
         <v>41</v>
@@ -17655,7 +17535,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="39" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="54"/>
       <c r="C39" s="41" t="s">
         <v>41</v>
@@ -17739,7 +17619,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="40" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="54"/>
       <c r="C40" s="41" t="s">
         <v>41</v>
@@ -17823,7 +17703,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="41" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="54"/>
       <c r="C41" s="41" t="s">
         <v>41</v>
@@ -17916,7 +17796,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="42" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="54"/>
       <c r="C42" s="41" t="s">
         <v>41</v>
@@ -18009,7 +17889,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="43" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="54"/>
       <c r="C43" s="41" t="s">
         <v>41</v>
@@ -18102,7 +17982,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="44" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="54"/>
       <c r="C44" s="41" t="s">
         <v>41</v>
@@ -18195,7 +18075,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="45" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="54"/>
       <c r="C45" s="41" t="s">
         <v>41</v>
@@ -18288,7 +18168,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="46" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="54"/>
       <c r="C46" s="41" t="s">
         <v>41</v>
@@ -18360,7 +18240,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="47" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="54"/>
       <c r="C47" s="41" t="s">
         <v>41</v>
@@ -18465,7 +18345,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="48" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="54"/>
       <c r="C48" s="41" t="s">
         <v>41</v>
@@ -18540,7 +18420,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="49" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="54"/>
       <c r="C49" s="41" t="s">
         <v>41</v>
@@ -18627,7 +18507,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="50" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="54"/>
       <c r="C50" s="41" t="s">
         <v>41</v>
@@ -18711,7 +18591,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="51" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="54"/>
       <c r="C51" s="41" t="s">
         <v>41</v>
@@ -18801,7 +18681,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="52" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="54"/>
       <c r="B52" s="41" t="s">
         <v>145</v>
@@ -18891,7 +18771,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="53" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="54"/>
       <c r="C53" s="41" t="s">
         <v>41</v>
@@ -18966,7 +18846,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="54" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="54"/>
       <c r="B54" s="41" t="s">
         <v>145</v>
@@ -19053,7 +18933,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="55" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="54"/>
       <c r="C55" s="41" t="s">
         <v>41</v>
@@ -19146,7 +19026,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="56" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="54"/>
       <c r="C56" s="41" t="s">
         <v>41</v>
@@ -19221,7 +19101,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="57" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="54"/>
       <c r="C57" s="41" t="s">
         <v>41</v>
@@ -19308,7 +19188,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="58" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="54"/>
       <c r="C58" s="41" t="s">
         <v>41</v>
@@ -19378,7 +19258,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="59" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="54"/>
       <c r="C59" s="41" t="s">
         <v>41</v>
@@ -19465,7 +19345,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="60" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="54"/>
       <c r="C60" s="41" t="s">
         <v>41</v>
@@ -19546,7 +19426,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="61" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="54"/>
       <c r="C61" s="41" t="s">
         <v>41</v>
@@ -19627,7 +19507,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="62" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="54"/>
       <c r="C62" s="41" t="s">
         <v>41</v>
@@ -19706,7 +19586,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="63" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="54"/>
       <c r="B63" s="41" t="s">
         <v>145</v>
@@ -19785,7 +19665,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="64" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="54"/>
       <c r="C64" s="41" t="s">
         <v>41</v>
@@ -19872,7 +19752,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="65" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="54"/>
       <c r="C65" s="41" t="s">
         <v>41</v>
@@ -19956,7 +19836,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="66" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="54"/>
       <c r="C66" s="41" t="s">
         <v>41</v>
@@ -20046,7 +19926,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="67" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="54"/>
       <c r="C67" s="41" t="s">
         <v>41</v>
@@ -20136,7 +20016,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="68" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="54"/>
       <c r="B68" s="41" t="s">
         <v>145</v>
@@ -20223,7 +20103,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="69" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="54"/>
       <c r="C69" s="41" t="s">
         <v>41</v>
@@ -20307,7 +20187,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="70" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="54"/>
       <c r="C70" s="41" t="s">
         <v>41</v>
@@ -20388,7 +20268,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="71" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="54"/>
       <c r="C71" s="41" t="s">
         <v>41</v>
@@ -20469,7 +20349,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="72" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="54"/>
       <c r="C72" s="41" t="s">
         <v>41</v>
@@ -20544,7 +20424,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="73" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="54"/>
       <c r="C73" s="41" t="s">
         <v>41</v>
@@ -20619,7 +20499,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="74" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="54"/>
       <c r="B74" s="41" t="s">
         <v>145</v>
@@ -20701,7 +20581,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="75" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="54"/>
       <c r="C75" s="41" t="s">
         <v>41</v>
@@ -20783,7 +20663,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="76" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="54"/>
       <c r="C76" s="41" t="s">
         <v>41</v>
@@ -20873,7 +20753,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="77" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="54"/>
       <c r="C77" s="41" t="s">
         <v>41</v>
@@ -20955,7 +20835,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="78" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="54"/>
       <c r="C78" s="41" t="s">
         <v>41</v>
@@ -21057,7 +20937,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="79" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="54"/>
       <c r="C79" s="41" t="s">
         <v>41</v>
@@ -21132,7 +21012,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="80" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="54"/>
       <c r="B80" s="41" t="s">
         <v>145</v>
@@ -21214,7 +21094,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="81" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="54"/>
       <c r="B81" s="41" t="s">
         <v>145</v>
@@ -21299,7 +21179,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="82" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="54"/>
       <c r="C82" s="41" t="s">
         <v>41</v>
@@ -21384,7 +21264,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="83" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="54"/>
       <c r="C83" s="41" t="s">
         <v>41</v>
@@ -21463,7 +21343,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="84" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="54"/>
       <c r="C84" s="41" t="s">
         <v>41</v>
@@ -21535,7 +21415,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="85" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="54"/>
       <c r="C85" s="41" t="s">
         <v>41</v>
@@ -21622,7 +21502,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="86" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="54"/>
       <c r="C86" s="41" t="s">
         <v>41</v>
@@ -21709,7 +21589,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="87" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="54"/>
       <c r="C87" s="41" t="s">
         <v>41</v>
@@ -21784,7 +21664,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="88" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="54"/>
       <c r="C88" s="41" t="s">
         <v>41</v>
@@ -21871,7 +21751,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="89" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="54"/>
       <c r="C89" s="41" t="s">
         <v>41</v>
@@ -21964,7 +21844,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="90" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="54"/>
       <c r="C90" s="41" t="s">
         <v>41</v>
@@ -22057,7 +21937,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="91" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="54"/>
       <c r="C91" s="41" t="s">
         <v>41</v>
@@ -22147,7 +22027,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="92" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="54"/>
       <c r="C92" s="41" t="s">
         <v>41</v>
@@ -22234,7 +22114,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="93" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="54"/>
       <c r="C93" s="41" t="s">
         <v>41</v>
@@ -22313,7 +22193,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="94" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="54"/>
       <c r="C94" s="41" t="s">
         <v>41</v>
@@ -22418,7 +22298,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="95" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="54"/>
       <c r="C95" s="41" t="s">
         <v>41</v>
@@ -22514,7 +22394,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="96" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="54"/>
       <c r="C96" s="41" t="s">
         <v>41</v>
@@ -22601,7 +22481,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="97" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="54"/>
       <c r="C97" s="41" t="s">
         <v>41</v>
@@ -22688,7 +22568,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="98" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="54"/>
       <c r="C98" s="41" t="s">
         <v>41</v>
@@ -22775,7 +22655,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="99" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="54"/>
       <c r="C99" s="41" t="s">
         <v>41</v>
@@ -22847,7 +22727,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="100" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="54"/>
       <c r="C100" s="41" t="s">
         <v>41</v>
@@ -22919,7 +22799,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="101" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="54"/>
       <c r="C101" s="41" t="s">
         <v>41</v>
@@ -22992,7 +22872,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="102" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="54"/>
       <c r="C102" s="41" t="s">
         <v>41</v>
@@ -23065,7 +22945,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="103" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="54"/>
       <c r="C103" s="41" t="s">
         <v>41</v>
@@ -23158,7 +23038,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="104" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="54"/>
       <c r="C104" s="41" t="s">
         <v>41</v>
@@ -23251,7 +23131,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="105" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="54"/>
       <c r="C105" s="41" t="s">
         <v>41</v>
@@ -23338,7 +23218,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="106" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="54"/>
       <c r="C106" s="41" t="s">
         <v>41</v>
@@ -23410,7 +23290,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="107" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="54"/>
       <c r="C107" s="41" t="s">
         <v>41</v>
@@ -23500,7 +23380,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="108" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="54"/>
       <c r="C108" s="41" t="s">
         <v>41</v>
@@ -23569,7 +23449,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="109" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="54"/>
       <c r="C109" s="41" t="s">
         <v>41</v>
@@ -23641,7 +23521,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="110" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="54"/>
       <c r="C110" s="41" t="s">
         <v>41</v>
@@ -23728,7 +23608,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="111" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="54"/>
       <c r="C111" s="41" t="s">
         <v>41</v>
@@ -23831,7 +23711,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="112" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="54"/>
       <c r="C112" s="41" t="s">
         <v>41</v>
@@ -23903,7 +23783,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="113" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="54"/>
       <c r="C113" s="41" t="s">
         <v>41</v>
@@ -23975,7 +23855,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="114" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="54"/>
       <c r="C114" s="41" t="s">
         <v>41</v>
@@ -24062,7 +23942,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="115" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="54"/>
       <c r="C115" s="41" t="s">
         <v>41</v>
@@ -24146,7 +24026,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="116" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="54"/>
       <c r="C116" s="41" t="s">
         <v>41</v>
@@ -24218,7 +24098,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="117" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="54"/>
       <c r="C117" s="41" t="s">
         <v>41</v>
@@ -24290,7 +24170,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="118" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="54"/>
       <c r="B118" s="41" t="s">
         <v>145</v>
@@ -24374,7 +24254,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="119" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="54"/>
       <c r="C119" s="41" t="s">
         <v>41</v>
@@ -24446,7 +24326,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="120" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="54"/>
       <c r="C120" s="41" t="s">
         <v>41</v>
@@ -24518,7 +24398,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="121" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="54"/>
       <c r="C121" s="41" t="s">
         <v>41</v>
@@ -24599,7 +24479,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="122" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="54"/>
       <c r="C122" s="41" t="s">
         <v>41</v>
@@ -24671,7 +24551,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="123" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="54"/>
       <c r="C123" s="41" t="s">
         <v>41</v>
@@ -24741,7 +24621,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="124" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="54"/>
       <c r="C124" s="41" t="s">
         <v>41</v>
@@ -24831,7 +24711,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="125" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="54"/>
       <c r="C125" s="41" t="s">
         <v>41</v>
@@ -24906,7 +24786,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="126" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="54"/>
       <c r="C126" s="41" t="s">
         <v>41</v>
@@ -24981,7 +24861,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="127" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="54"/>
       <c r="C127" s="41" t="s">
         <v>41</v>
@@ -25071,7 +24951,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="128" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="54"/>
       <c r="C128" s="41" t="s">
         <v>41</v>
@@ -25164,7 +25044,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="129" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="54"/>
       <c r="C129" s="41" t="s">
         <v>41</v>
@@ -25257,7 +25137,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="130" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="54"/>
       <c r="C130" s="41" t="s">
         <v>41</v>
@@ -25338,7 +25218,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="131" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="54"/>
       <c r="C131" s="41" t="s">
         <v>41</v>
@@ -25434,7 +25314,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="132" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="54"/>
       <c r="C132" s="41" t="s">
         <v>41</v>
@@ -25527,7 +25407,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="133" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="54"/>
       <c r="C133" s="41" t="s">
         <v>41</v>
@@ -25620,7 +25500,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="134" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="54"/>
       <c r="C134" s="41" t="s">
         <v>41</v>
@@ -25719,7 +25599,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="135" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="54"/>
       <c r="B135" s="41" t="s">
         <v>145</v>
@@ -25810,7 +25690,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="136" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="54"/>
       <c r="C136" s="41" t="s">
         <v>41</v>
@@ -25898,7 +25778,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="137" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="54"/>
       <c r="C137" s="41" t="s">
         <v>41</v>
@@ -26003,7 +25883,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="138" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="54"/>
       <c r="C138" s="41" t="s">
         <v>41</v>
@@ -26084,7 +25964,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="139" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="54"/>
       <c r="C139" s="41" t="s">
         <v>41</v>
@@ -26177,7 +26057,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="140" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="54"/>
       <c r="C140" s="41" t="s">
         <v>41</v>
@@ -26261,7 +26141,7 @@
         <v>3247</v>
       </c>
     </row>
-    <row r="141" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="54"/>
       <c r="C141" s="41" t="s">
         <v>41</v>
@@ -26345,7 +26225,7 @@
         <v>3248</v>
       </c>
     </row>
-    <row r="142" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="54"/>
       <c r="C142" s="41" t="s">
         <v>41</v>
@@ -26421,7 +26301,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="143" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="54"/>
       <c r="C143" s="41" t="s">
         <v>41</v>
@@ -26503,7 +26383,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="144" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="54"/>
       <c r="C144" s="41" t="s">
         <v>41</v>
@@ -26599,7 +26479,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="145" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="54"/>
       <c r="C145" s="41" t="s">
         <v>41</v>
@@ -26681,7 +26561,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="146" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="54"/>
       <c r="C146" s="41" t="s">
         <v>41</v>
@@ -26762,7 +26642,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="147" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="54"/>
       <c r="B147" s="41" t="s">
         <v>145</v>
@@ -26849,7 +26729,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="148" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="54"/>
       <c r="C148" s="41" t="s">
         <v>41</v>
@@ -26933,7 +26813,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="149" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="54"/>
       <c r="C149" s="41" t="s">
         <v>41</v>
@@ -27014,7 +26894,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="150" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="54"/>
       <c r="C150" s="41" t="s">
         <v>41</v>
@@ -27125,7 +27005,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="151" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="54"/>
       <c r="C151" s="41" t="s">
         <v>41</v>
@@ -27233,7 +27113,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="152" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="54"/>
       <c r="C152" s="41" t="s">
         <v>41</v>
@@ -27323,7 +27203,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="153" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="54"/>
       <c r="C153" s="41" t="s">
         <v>41</v>
@@ -27398,7 +27278,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="154" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="54"/>
       <c r="C154" s="41" t="s">
         <v>41</v>
@@ -27476,7 +27356,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="155" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="54"/>
       <c r="C155" s="41" t="s">
         <v>41</v>
@@ -27581,7 +27461,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="156" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="54"/>
       <c r="C156" s="41" t="s">
         <v>41</v>
@@ -27668,7 +27548,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="157" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="54"/>
       <c r="C157" s="41" t="s">
         <v>41</v>
@@ -27743,7 +27623,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="158" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="54"/>
       <c r="C158" s="41" t="s">
         <v>41</v>
@@ -27824,7 +27704,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="159" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="54"/>
       <c r="C159" s="41" t="s">
         <v>41</v>
@@ -27917,7 +27797,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="160" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="54"/>
       <c r="C160" s="41" t="s">
         <v>41</v>
@@ -28001,7 +27881,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="161" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="54"/>
       <c r="C161" s="41" t="s">
         <v>41</v>
@@ -28073,7 +27953,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="162" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="54"/>
       <c r="C162" s="41" t="s">
         <v>41</v>
@@ -28145,7 +28025,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="163" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="54"/>
       <c r="C163" s="41" t="s">
         <v>41</v>
@@ -28238,7 +28118,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="164" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="54"/>
       <c r="C164" s="41" t="s">
         <v>41</v>
@@ -28352,7 +28232,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="165" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="54"/>
       <c r="B165" s="41" t="s">
         <v>145</v>
@@ -28448,7 +28328,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="166" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="54"/>
       <c r="B166" s="41" t="s">
         <v>145</v>
@@ -28541,7 +28421,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="167" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="54"/>
       <c r="C167" s="41" t="s">
         <v>41</v>
@@ -28649,7 +28529,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="168" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="54"/>
       <c r="C168" s="41" t="s">
         <v>41</v>
@@ -28757,7 +28637,7 @@
         <v>3266</v>
       </c>
     </row>
-    <row r="169" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="54"/>
       <c r="C169" s="41" t="s">
         <v>41</v>
@@ -28847,7 +28727,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="170" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="54"/>
       <c r="C170" s="41" t="s">
         <v>41</v>
@@ -28937,7 +28817,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="171" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="54"/>
       <c r="C171" s="41" t="s">
         <v>41</v>
@@ -29019,7 +28899,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="172" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="54"/>
       <c r="C172" s="41" t="s">
         <v>41</v>
@@ -29109,7 +28989,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="173" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="54"/>
       <c r="C173" s="41" t="s">
         <v>41</v>
@@ -29193,7 +29073,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="174" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="54"/>
       <c r="C174" s="41" t="s">
         <v>41</v>
@@ -29283,7 +29163,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="175" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="54"/>
       <c r="C175" s="41" t="s">
         <v>41</v>
@@ -29355,7 +29235,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="176" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="54"/>
       <c r="C176" s="41" t="s">
         <v>41</v>
@@ -29436,7 +29316,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="177" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="54"/>
       <c r="C177" s="41" t="s">
         <v>41</v>
@@ -29517,7 +29397,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="178" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="54"/>
       <c r="B178" s="41" t="s">
         <v>145</v>
@@ -29598,7 +29478,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="179" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="54"/>
       <c r="C179" s="41" t="s">
         <v>41</v>
@@ -29682,7 +29562,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="180" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="54"/>
       <c r="C180" s="41" t="s">
         <v>41</v>
@@ -29766,7 +29646,7 @@
         <v>3267</v>
       </c>
     </row>
-    <row r="181" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="54"/>
       <c r="C181" s="41" t="s">
         <v>41</v>
@@ -29862,7 +29742,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="182" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="54"/>
       <c r="C182" s="41" t="s">
         <v>41</v>
@@ -29949,7 +29829,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="183" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="54"/>
       <c r="C183" s="41" t="s">
         <v>41</v>
@@ -30021,7 +29901,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="184" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="54"/>
       <c r="C184" s="41" t="s">
         <v>41</v>
@@ -30111,7 +29991,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="185" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="54"/>
       <c r="C185" s="41" t="s">
         <v>41</v>
@@ -30186,7 +30066,7 @@
         <v>2033</v>
       </c>
     </row>
-    <row r="186" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="54"/>
       <c r="B186" s="41" t="s">
         <v>145</v>
@@ -30279,7 +30159,7 @@
         <v>2033</v>
       </c>
     </row>
-    <row r="187" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="54"/>
       <c r="C187" s="41" t="s">
         <v>41</v>
@@ -30384,7 +30264,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="188" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="54"/>
       <c r="C188" s="41" t="s">
         <v>41</v>
@@ -30471,7 +30351,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="189" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="54"/>
       <c r="C189" s="41" t="s">
         <v>41</v>
@@ -30558,7 +30438,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="190" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="54"/>
       <c r="C190" s="41" t="s">
         <v>41</v>
@@ -30636,7 +30516,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="191" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="54"/>
       <c r="C191" s="41" t="s">
         <v>41</v>
@@ -30711,7 +30591,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="192" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="54"/>
       <c r="C192" s="41" t="s">
         <v>41</v>
@@ -30777,7 +30657,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="193" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="54"/>
       <c r="C193" s="41" t="s">
         <v>41</v>
@@ -30882,7 +30762,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="194" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="54"/>
       <c r="C194" s="41" t="s">
         <v>41</v>
@@ -30957,7 +30837,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="195" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="54"/>
       <c r="C195" s="41" t="s">
         <v>41</v>
@@ -31062,7 +30942,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="196" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="54"/>
       <c r="C196" s="41" t="s">
         <v>41</v>
@@ -31137,7 +31017,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="197" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="54"/>
       <c r="C197" s="41" t="s">
         <v>41</v>
@@ -31206,7 +31086,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="198" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="54"/>
       <c r="C198" s="41" t="s">
         <v>41</v>
@@ -31293,7 +31173,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="199" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="54"/>
       <c r="C199" s="41" t="s">
         <v>41</v>
@@ -31380,7 +31260,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="200" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="54"/>
       <c r="C200" s="41" t="s">
         <v>41</v>
@@ -31452,7 +31332,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="201" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="54"/>
       <c r="C201" s="41" t="s">
         <v>41</v>
@@ -31533,7 +31413,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="202" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="54"/>
       <c r="C202" s="41" t="s">
         <v>41</v>
@@ -31620,7 +31500,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="203" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="54"/>
       <c r="C203" s="41" t="s">
         <v>41</v>
@@ -31692,7 +31572,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="204" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="54"/>
       <c r="C204" s="41" t="s">
         <v>41</v>
@@ -31773,7 +31653,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="205" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="54"/>
       <c r="C205" s="41" t="s">
         <v>41</v>
@@ -31845,7 +31725,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="206" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="54"/>
       <c r="C206" s="41" t="s">
         <v>41</v>
@@ -31932,7 +31812,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="207" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="54"/>
       <c r="C207" s="41" t="s">
         <v>41</v>
@@ -32011,7 +31891,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="208" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="54"/>
       <c r="C208" s="41" t="s">
         <v>41</v>
@@ -32096,7 +31976,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="209" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="54"/>
       <c r="C209" s="41" t="s">
         <v>41</v>
@@ -32186,7 +32066,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="210" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="54"/>
       <c r="C210" s="41" t="s">
         <v>41</v>
@@ -32267,7 +32147,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="211" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="54"/>
       <c r="C211" s="41" t="s">
         <v>41</v>
@@ -32363,7 +32243,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="212" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="54"/>
       <c r="C212" s="41" t="s">
         <v>41</v>
@@ -32465,7 +32345,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="213" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="54"/>
       <c r="C213" s="41" t="s">
         <v>41</v>
@@ -32552,7 +32432,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="214" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="54"/>
       <c r="C214" s="41" t="s">
         <v>41</v>
@@ -32642,7 +32522,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="215" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="54"/>
       <c r="C215" s="41" t="s">
         <v>41</v>
@@ -32732,7 +32612,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="216" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="54"/>
       <c r="C216" s="41" t="s">
         <v>41</v>
@@ -32810,7 +32690,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="217" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="54"/>
       <c r="C217" s="41" t="s">
         <v>41</v>
@@ -32882,7 +32762,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="218" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="54"/>
       <c r="C218" s="41" t="s">
         <v>41</v>
@@ -32975,7 +32855,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="219" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="54"/>
       <c r="C219" s="41" t="s">
         <v>41</v>
@@ -33062,7 +32942,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="220" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="54"/>
       <c r="C220" s="41" t="s">
         <v>41</v>
@@ -33137,7 +33017,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="221" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="54"/>
       <c r="C221" s="41" t="s">
         <v>41</v>
@@ -33227,7 +33107,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="222" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="54"/>
       <c r="C222" s="41" t="s">
         <v>41</v>
@@ -33311,7 +33191,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="223" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="54"/>
       <c r="C223" s="41" t="s">
         <v>41</v>
@@ -33401,7 +33281,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="224" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="54"/>
       <c r="C224" s="41" t="s">
         <v>41</v>
@@ -33494,7 +33374,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="225" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="54"/>
       <c r="C225" s="41" t="s">
         <v>41</v>
@@ -33587,7 +33467,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="226" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="54"/>
       <c r="C226" s="41" t="s">
         <v>41</v>
@@ -33680,7 +33560,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="227" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="54"/>
       <c r="C227" s="41" t="s">
         <v>41</v>
@@ -33770,7 +33650,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="228" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="54"/>
       <c r="C228" s="41" t="s">
         <v>41</v>
@@ -33845,7 +33725,7 @@
         <v>3976</v>
       </c>
     </row>
-    <row r="229" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="54"/>
       <c r="C229" s="41" t="s">
         <v>41</v>
@@ -33938,7 +33818,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="230" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="54"/>
       <c r="C230" s="41" t="s">
         <v>41</v>
@@ -34028,7 +33908,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="231" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="54"/>
       <c r="C231" s="41" t="s">
         <v>41</v>
@@ -34109,7 +33989,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="232" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="54"/>
       <c r="C232" s="41" t="s">
         <v>41</v>
@@ -34190,7 +34070,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="233" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="54"/>
       <c r="C233" s="41" t="s">
         <v>41</v>
@@ -34274,7 +34154,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="234" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" s="54"/>
       <c r="C234" s="41" t="s">
         <v>41</v>
@@ -34340,7 +34220,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="235" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="54"/>
       <c r="C235" s="41" t="s">
         <v>41</v>
@@ -34410,7 +34290,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="236" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" s="54"/>
       <c r="C236" s="41" t="s">
         <v>41</v>
@@ -34482,7 +34362,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="237" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" s="54"/>
       <c r="C237" s="41" t="s">
         <v>41</v>
@@ -34563,7 +34443,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="238" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" s="54"/>
       <c r="C238" s="41" t="s">
         <v>41</v>
@@ -34665,7 +34545,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="239" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="54"/>
       <c r="C239" s="41" t="s">
         <v>41</v>
@@ -34770,7 +34650,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="240" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A240" s="54"/>
       <c r="C240" s="41" t="s">
         <v>41</v>
@@ -34857,7 +34737,7 @@
         <v>3278</v>
       </c>
     </row>
-    <row r="241" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" s="54"/>
       <c r="C241" s="41" t="s">
         <v>41</v>
@@ -34947,7 +34827,7 @@
         <v>3279</v>
       </c>
     </row>
-    <row r="242" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A242" s="54"/>
       <c r="C242" s="41" t="s">
         <v>41</v>
@@ -35034,7 +34914,7 @@
         <v>3279</v>
       </c>
     </row>
-    <row r="243" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A243" s="54"/>
       <c r="C243" s="41" t="s">
         <v>41</v>
@@ -35121,7 +35001,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="244" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A244" s="54"/>
       <c r="C244" s="41" t="s">
         <v>41</v>
@@ -35214,7 +35094,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="245" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A245" s="54"/>
       <c r="C245" s="41" t="s">
         <v>41</v>
@@ -35307,7 +35187,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="246" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" s="54"/>
       <c r="C246" s="41" t="s">
         <v>41</v>
@@ -35400,7 +35280,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="247" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A247" s="54"/>
       <c r="C247" s="41" t="s">
         <v>41</v>
@@ -35493,7 +35373,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="248" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A248" s="54"/>
       <c r="C248" s="41" t="s">
         <v>41</v>
@@ -35583,7 +35463,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="249" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A249" s="54"/>
       <c r="C249" s="41" t="s">
         <v>41</v>
@@ -35688,7 +35568,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="250" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" s="54"/>
       <c r="C250" s="41" t="s">
         <v>41</v>
@@ -35775,7 +35655,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="251" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" s="54"/>
       <c r="C251" s="41" t="s">
         <v>41</v>
@@ -35877,7 +35757,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="252" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A252" s="54"/>
       <c r="C252" s="41" t="s">
         <v>41</v>
@@ -35964,7 +35844,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="253" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A253" s="54"/>
       <c r="C253" s="41" t="s">
         <v>41</v>
@@ -36051,7 +35931,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="254" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A254" s="54"/>
       <c r="C254" s="41" t="s">
         <v>41</v>
@@ -36126,7 +36006,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="255" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A255" s="54"/>
       <c r="C255" s="41" t="s">
         <v>41</v>
@@ -36210,7 +36090,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="256" spans="1:49" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:49" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A256" s="54"/>
       <c r="C256" s="41" t="s">
         <v>41</v>
@@ -36297,7 +36177,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="257" spans="1:50" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:50" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A257" s="54"/>
       <c r="C257" s="41" t="s">
         <v>41</v>
@@ -36384,7 +36264,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="258" spans="1:50" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:50" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="54"/>
       <c r="C258" s="41" t="s">
         <v>41</v>
@@ -36471,7 +36351,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="259" spans="1:50" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:50" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="54"/>
       <c r="C259" s="41" t="s">
         <v>41</v>
@@ -36558,7 +36438,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="260" spans="1:50" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:50" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A260" s="54"/>
       <c r="C260" s="41" t="s">
         <v>41</v>
@@ -36648,7 +36528,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="261" spans="1:50" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:50" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A261" s="54"/>
       <c r="C261" s="41" t="s">
         <v>41</v>
@@ -36738,7 +36618,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="262" spans="1:50" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:50" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A262" s="54"/>
       <c r="C262" s="41" t="s">
         <v>41</v>
@@ -36843,7 +36723,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="263" spans="1:50" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:50" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A263" s="54"/>
       <c r="C263" s="41" t="s">
         <v>41</v>
@@ -36936,7 +36816,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="264" spans="1:50" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:50" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A264" s="54"/>
       <c r="C264" s="41" t="s">
         <v>41</v>
@@ -37023,7 +36903,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="265" spans="1:50" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:50" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A265" s="54"/>
       <c r="C265" s="41" t="s">
         <v>41</v>
@@ -37110,7 +36990,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="266" spans="1:50" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:50" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A266" s="54"/>
       <c r="C266" s="41" t="s">
         <v>41</v>
@@ -37203,7 +37083,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="267" spans="1:50" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:50" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A267" s="54"/>
       <c r="C267" s="41" t="s">
         <v>41</v>
@@ -37296,7 +37176,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="268" spans="1:50" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:50" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A268" s="54"/>
       <c r="C268" s="41" t="s">
         <v>41</v>
@@ -37383,7 +37263,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="269" spans="1:50" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:50" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A269" s="54"/>
       <c r="C269" s="41" t="s">
         <v>41</v>
@@ -37473,7 +37353,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="270" spans="1:50" s="41" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:50" s="41" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A270" s="54"/>
       <c r="C270" s="41" t="s">
         <v>41</v>
@@ -37572,7 +37452,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="271" spans="1:50" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:50" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A271" s="56"/>
       <c r="B271" s="56"/>
       <c r="C271" s="56"/>
@@ -37624,7 +37504,7 @@
       <c r="AW271" s="56"/>
       <c r="AX271" s="56"/>
     </row>
-    <row r="272" spans="1:50" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:50" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A272" s="56"/>
       <c r="B272" s="56"/>
       <c r="C272" s="56"/>
@@ -37676,7 +37556,7 @@
       <c r="AW272" s="56"/>
       <c r="AX272" s="56"/>
     </row>
-    <row r="273" spans="1:50" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:50" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A273" s="56"/>
       <c r="B273" s="56"/>
       <c r="C273" s="56"/>
@@ -37728,7 +37608,7 @@
       <c r="AW273" s="56"/>
       <c r="AX273" s="56"/>
     </row>
-    <row r="274" spans="1:50" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:50" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A274" s="56"/>
       <c r="B274" s="56"/>
       <c r="C274" s="56"/>
@@ -37780,7 +37660,7 @@
       <c r="AW274" s="56"/>
       <c r="AX274" s="56"/>
     </row>
-    <row r="275" spans="1:50" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:50" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A275" s="56"/>
       <c r="B275" s="56"/>
       <c r="C275" s="56"/>
@@ -37832,7 +37712,7 @@
       <c r="AW275" s="56"/>
       <c r="AX275" s="56"/>
     </row>
-    <row r="276" spans="1:50" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:50" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A276" s="56"/>
       <c r="B276" s="56"/>
       <c r="C276" s="56"/>
@@ -37884,7 +37764,7 @@
       <c r="AW276" s="56"/>
       <c r="AX276" s="56"/>
     </row>
-    <row r="277" spans="1:50" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:50" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A277" s="56"/>
       <c r="B277" s="56"/>
       <c r="C277" s="56"/>
@@ -37936,7 +37816,7 @@
       <c r="AW277" s="56"/>
       <c r="AX277" s="56"/>
     </row>
-    <row r="278" spans="1:50" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:50" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A278" s="56"/>
       <c r="B278" s="56"/>
       <c r="C278" s="56"/>
@@ -37988,7 +37868,7 @@
       <c r="AW278" s="56"/>
       <c r="AX278" s="56"/>
     </row>
-    <row r="279" spans="1:50" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:50" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A279" s="56"/>
       <c r="B279" s="56"/>
       <c r="C279" s="56"/>
@@ -38040,7 +37920,7 @@
       <c r="AW279" s="56"/>
       <c r="AX279" s="56"/>
     </row>
-    <row r="280" spans="1:50" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:50" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A280" s="56"/>
       <c r="B280" s="56"/>
       <c r="C280" s="56"/>
@@ -38092,7 +37972,7 @@
       <c r="AW280" s="56"/>
       <c r="AX280" s="56"/>
     </row>
-    <row r="281" spans="1:50" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:50" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A281" s="56"/>
       <c r="B281" s="56"/>
       <c r="C281" s="56"/>
@@ -38144,7 +38024,7 @@
       <c r="AW281" s="56"/>
       <c r="AX281" s="56"/>
     </row>
-    <row r="282" spans="1:50" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:50" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A282" s="56"/>
       <c r="B282" s="56"/>
       <c r="C282" s="56"/>
@@ -38196,7 +38076,7 @@
       <c r="AW282" s="56"/>
       <c r="AX282" s="56"/>
     </row>
-    <row r="283" spans="1:50" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:50" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A283" s="56"/>
       <c r="B283" s="56"/>
       <c r="C283" s="56"/>
@@ -38248,7 +38128,7 @@
       <c r="AW283" s="56"/>
       <c r="AX283" s="56"/>
     </row>
-    <row r="284" spans="1:50" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:50" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A284" s="56"/>
       <c r="B284" s="56"/>
       <c r="C284" s="56"/>
@@ -38304,42 +38184,37 @@
   <autoFilter ref="A1:AZ286"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="H271:H1048576">
-    <cfRule type="duplicateValues" dxfId="19" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G271:G1048576">
-    <cfRule type="duplicateValues" dxfId="18" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q271:Q1048576">
-    <cfRule type="duplicateValues" dxfId="17" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R271:R1048576">
-    <cfRule type="duplicateValues" dxfId="16" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR271:AR1048576">
-    <cfRule type="duplicateValues" dxfId="15" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q271:Q1048576">
-    <cfRule type="duplicateValues" dxfId="14" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R271:R1048576">
-    <cfRule type="duplicateValues" dxfId="13" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="S271:S1048576">
-    <cfRule type="duplicateValues" dxfId="12" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M271:M1048576">
-    <cfRule type="duplicateValues" dxfId="11" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="W271:W1048576">
-    <cfRule type="duplicateValues" dxfId="10" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="8"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>